<commit_message>
add a test case for ZSS-1391
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/merge/book/1390-mergedHidden.xlsx
+++ b/zss.test/src/main/webapp/merge/book/1390-mergedHidden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zkspreadsheet/zss.test/src/main/webapp/merge/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA18DAC6-26B8-8144-BA39-9421A6A4A997}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F4D95D-E040-6B48-8A15-09D6505D6EF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{8A517463-96FA-C64D-BFFC-EB417987D631}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>merged
 F5: F8</t>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>merge A3:C3 and hidden</t>
+  </si>
+  <si>
+    <t>right alignment</t>
+  </si>
+  <si>
+    <t>vertical center</t>
   </si>
 </sst>
 </file>
@@ -73,14 +79,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,64 +409,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6935ED-9534-534D-963E-EA952D758674}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I5" sqref="I5:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F5" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="H5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="A11:C11"/>
     <mergeCell ref="G5:G8"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>

</xml_diff>